<commit_message>
Updated R code and metadata file
</commit_message>
<xml_diff>
--- a/Radar_metadata.xlsx
+++ b/Radar_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\312202_visavis\WP2\Previous_radar_migration\Old_radar_data_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\312202_visavis\WP2\Previous_radar_migration\old_radar_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028536B7-DDC3-4472-AFBC-8A199EFAF744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C958720-F00D-4C65-86FB-203A924C924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="3015" windowWidth="23250" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Location</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Other databases</t>
+  </si>
+  <si>
+    <t>m201608; m201609; m201610</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -265,9 +268,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,8 +665,31 @@
       <c r="D4" t="s">
         <v>50</v>
       </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="I4" s="5">
+        <v>42673</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -923,33 +946,33 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="9" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E16" s="7" t="s">
+      <c r="E16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="7" t="s">
+      <c r="E17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="7" t="s">
+      <c r="E18" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>